<commit_message>
Improve talent submission logging and error handling
Added detailed logging of submission details in ABpedro_talent_submission_update.py for better traceability. Refactored talent_submit view to simplify submission logic, improve error messages, and ensure submissions are saved and sent to Discord with clearer success and failure responses.
</commit_message>
<xml_diff>
--- a/pedroproject/Atalent_submissions.xlsx
+++ b/pedroproject/Atalent_submissions.xlsx
@@ -1331,12 +1331,12 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Injective Supporter</t>
+          <t>None</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>3-5 years</t>
+          <t>&lt;1 year</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -1346,7 +1346,7 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Switzerland</t>
+          <t>Portugal</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
@@ -1356,12 +1356,12 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>Custom Rate</t>
+          <t>$0-$500</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>Solidity</t>
+          <t>Rust, DAO Contributor</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
@@ -1416,7 +1416,7 @@
       </c>
       <c r="T8" t="inlineStr">
         <is>
-          <t>1697944</t>
+          <t>1697931</t>
         </is>
       </c>
       <c r="U8" t="inlineStr">
@@ -1441,12 +1441,12 @@
       </c>
       <c r="Y8" t="inlineStr">
         <is>
-          <t>2025-12-19 00:47:05</t>
+          <t>2025-12-19 10:13:32</t>
         </is>
       </c>
       <c r="Z8" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Queued</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Refactor Discord bot to use Excel as single source of truth
Major refactor to remove in-memory submission queues and use the Excel file as the authoritative source for all submission status and data. Adds helper methods for filtering and counting submissions by status, and updates all commands to operate directly on the Excel file. The review workflow now uses the 'Pending' status, and only approved submissions are shown in the public list. Improves error handling, code structure, and documentation throughout.
</commit_message>
<xml_diff>
--- a/pedroproject/Atalent_submissions.xlsx
+++ b/pedroproject/Atalent_submissions.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="1900" yWindow="1900" windowWidth="19200" windowHeight="11170" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Submissions" sheetId="1" state="visible" r:id="rId1"/>
@@ -414,8 +414,8 @@
   </sheetPr>
   <dimension ref="A1:Z8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
-      <selection activeCell="T8" sqref="A8:XFD8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
@@ -1331,7 +1331,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Injective Supporter</t>
+          <t>Injective Community Artist</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -1346,7 +1346,7 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Spain</t>
+          <t>Finland</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
@@ -1356,17 +1356,17 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>$1,000-$2,500</t>
+          <t>$0-$500</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>Solidity</t>
+          <t>Move</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>Spanish</t>
+          <t>Ukrainian</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
@@ -1416,7 +1416,7 @@
       </c>
       <c r="T8" t="inlineStr">
         <is>
-          <t>1697927</t>
+          <t>1697921</t>
         </is>
       </c>
       <c r="U8" t="inlineStr">
@@ -1436,17 +1436,17 @@
       </c>
       <c r="X8" t="inlineStr">
         <is>
-          <t>aaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaa</t>
+          <t>aaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaa</t>
         </is>
       </c>
       <c r="Y8" t="inlineStr">
         <is>
-          <t>2025-12-19 10:59:51</t>
+          <t>2025-12-19 15:39:15</t>
         </is>
       </c>
       <c r="Z8" t="inlineStr">
         <is>
-          <t>Queued</t>
+          <t>Pending</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Enhance Discord bot submission review workflow
Major refactor and feature expansion for the Discord TalentHubBot: adds quick approve/review actions, improved notification embeds, periodic reminders, and robust queue handling for submissions. Bot startup and threading logic are improved for Django compatibility, and the submission review UI is streamlined for better usability. Also updates Excel handling and error management throughout the bot workflow.
</commit_message>
<xml_diff>
--- a/pedroproject/Atalent_submissions.xlsx
+++ b/pedroproject/Atalent_submissions.xlsx
@@ -412,7 +412,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Z8"/>
+  <dimension ref="A1:AA8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A8" sqref="A8:XFD8"/>
@@ -551,6 +551,11 @@
           <t>Status</t>
         </is>
       </c>
+      <c r="AA1" t="inlineStr">
+        <is>
+          <t>Test Write</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -1446,7 +1451,7 @@
       </c>
       <c r="Z8" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Approved</t>
         </is>
       </c>
     </row>

</xml_diff>